<commit_message>
Rename PFRCost as REGCV1Cost for clarification
</commit_message>
<xml_diff>
--- a/ams/cases/ieee123/ieee123_regcv1.xlsx
+++ b/ams/cases/ieee123/ieee123_regcv1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee123/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAB8523-BB6D-3342-A061-39F58B460EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B51E32B-1817-8240-9770-103061017F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="16" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Slack" sheetId="4" r:id="rId5"/>
     <sheet name="Line" sheetId="5" r:id="rId6"/>
     <sheet name="GCost" sheetId="14" r:id="rId7"/>
-    <sheet name="PFRCost" sheetId="15" r:id="rId8"/>
+    <sheet name="REGCV1Cost" sheetId="15" r:id="rId8"/>
     <sheet name="REGCV1" sheetId="17" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -19918,8 +19918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30096DF9-AE9D-C146-865B-1CF57605739C}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20141,7 +20141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419D3FAE-44DF-2C46-8059-BFA4F80E21D4}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>

</xml_diff>